<commit_message>
ut-2: conceptual model much simplified and ut-queries.
</commit_message>
<xml_diff>
--- a/06-MorMee_Constraints/MorMee-PowerConstraints.xlsx
+++ b/06-MorMee_Constraints/MorMee-PowerConstraints.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="77">
   <si>
     <t>Cardinality</t>
   </si>
@@ -74,9 +74,6 @@
     <t>skos:Concept</t>
   </si>
   <si>
-    <t>FINANCIAL</t>
-  </si>
-  <si>
     <t>AmountType</t>
   </si>
   <si>
@@ -107,9 +104,6 @@
     <t>[Subcriterion Description]</t>
   </si>
   <si>
-    <t>List of the EU MS countries where a Legal or Natural Person can act</t>
-  </si>
-  <si>
     <t>Comments</t>
   </si>
   <si>
@@ -134,12 +128,6 @@
     <t>NUTS-2016</t>
   </si>
   <si>
-    <t>b033b149-aa22-49e3-8c96-b1a9132c8456</t>
-  </si>
-  <si>
-    <t>currencyId compulsory</t>
-  </si>
-  <si>
     <t>PeriodType</t>
   </si>
   <si>
@@ -161,18 +149,12 @@
     <t>URI</t>
   </si>
   <si>
-    <t>https://github.com/everis-rpam/RPaM-Ontology/blob/v1.1.0/06-MorMee_Constraints/mormeeconstraints.ttl#MaxPaymentThresholdConstraint</t>
-  </si>
-  <si>
     <t>GenericConstraints</t>
   </si>
   <si>
     <t>Group of usual constraints expressed in a very generic way.</t>
   </si>
   <si>
-    <t>GENERIC</t>
-  </si>
-  <si>
     <t>https://github.com/everis-rpam/RPaM-Ontology/blob/v1.1.0/06-MorMee_Constraints/mormeeconstraints.ttl#GenericConstraint</t>
   </si>
   <si>
@@ -188,45 +170,12 @@
     <t>725c8a75-74f2-4cae-b1f6-11a82400f6d9</t>
   </si>
   <si>
-    <t>https://github.com/everis-rpam/RPaM-Ontology/blob/v1.1.0/06-MorMee_Constraints/mormeeconstraints.ttl#GenericGroup</t>
-  </si>
-  <si>
-    <t>https://github.com/everis-rpam/RPaM-Ontology/blob/v1.1.0/06-MorMee_Constraints/mormeeconstraints.ttl#FinancialConstraintProperty</t>
-  </si>
-  <si>
-    <t>https://github.com/everis-rpam/RPaM-Ontology/blob/v1.1.0/06-MorMee_Constraints/mormeeconstraints.ttl#GeographicalConstraintProperty</t>
-  </si>
-  <si>
-    <t>https://github.com/everis-rpam/RPaM-Ontology/blob/v1.1.0/06-MorMee_Constraints/mormeeconstraints.ttl#ValidityPeriodConstraintProperty</t>
-  </si>
-  <si>
-    <t>TERRITORIAL_UNIT</t>
-  </si>
-  <si>
-    <t>Territorial Unit</t>
-  </si>
-  <si>
     <t>Constraints applied to the use of powers by mandators and mandatees. Rule: the statements are to be expressed always in a negative form. Please bear in mind this rule when defining new constraints.</t>
   </si>
   <si>
-    <t>FINANCIAL CEIL</t>
-  </si>
-  <si>
-    <t>Financial Ceil</t>
-  </si>
-  <si>
     <t>The person cannot use the power above the amount of</t>
   </si>
   <si>
-    <t>The person can not use the power in the following territorial units</t>
-  </si>
-  <si>
-    <t>VALIDITY_PERIOD</t>
-  </si>
-  <si>
-    <t>Validity Period</t>
-  </si>
-  <si>
     <t>If a measure is used to express the length of the period: 1) the endDate must not be specified; and 2) the unitCode of the measure must be specified.</t>
   </si>
   <si>
@@ -243,6 +192,66 @@
   </si>
   <si>
     <t>[e.g. startDate = 2019-01-01, 3 YEAR]</t>
+  </si>
+  <si>
+    <t>List of basic generic constraints</t>
+  </si>
+  <si>
+    <t>Territorial unit scope</t>
+  </si>
+  <si>
+    <t>Financial ceil</t>
+  </si>
+  <si>
+    <t>The person can not use the power out of the following territorial unit(s)</t>
+  </si>
+  <si>
+    <t>One single use</t>
+  </si>
+  <si>
+    <t>The person cannot use the power more than once</t>
+  </si>
+  <si>
+    <t>IndicatorType</t>
+  </si>
+  <si>
+    <t>Once successfully consumed the power, the SP must notify the eMandate Registry so the Registry can change the status of the power.</t>
+  </si>
+  <si>
+    <t>Compulsory use of NUTs for the identification of territorial units</t>
+  </si>
+  <si>
+    <t>Attribute `currencyId` compulsory when the value is an amount</t>
+  </si>
+  <si>
+    <t>[e.g. true]</t>
+  </si>
+  <si>
+    <t>If `true`, the maximum number of uses is 1, otherwise it is unlimited</t>
+  </si>
+  <si>
+    <t>xsd:boolean</t>
+  </si>
+  <si>
+    <t>OneSingleUse</t>
+  </si>
+  <si>
+    <t>ValidityPeriodConstraint</t>
+  </si>
+  <si>
+    <t>TerritorialUnitScope</t>
+  </si>
+  <si>
+    <t>FinancialCeil</t>
+  </si>
+  <si>
+    <t>GenericConstraintsGroup</t>
+  </si>
+  <si>
+    <t>Validity period</t>
+  </si>
+  <si>
+    <t>GenericConstraintCriterion</t>
   </si>
 </sst>
 </file>
@@ -795,7 +804,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -914,6 +923,9 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="44">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1247,12 +1259,12 @@
   <sheetData>
     <row r="4" spans="3:3" x14ac:dyDescent="0.45">
       <c r="C4" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="3:3" x14ac:dyDescent="0.45">
       <c r="C5" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -1262,13 +1274,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD73"/>
+  <dimension ref="A1:AD74"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomRight" activeCell="R10" sqref="R10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.46484375" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1280,8 +1292,8 @@
     <col min="9" max="9" width="2.796875" style="2" hidden="1" customWidth="1"/>
     <col min="10" max="16" width="3.796875" style="2" hidden="1" customWidth="1"/>
     <col min="17" max="17" width="19.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="55.86328125" style="2" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="15.796875" style="13" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="57.86328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="21.9296875" style="13" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="11.9296875" style="2" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="14.796875" style="2" customWidth="1"/>
     <col min="22" max="22" width="10.53125" style="13" bestFit="1" customWidth="1"/>
@@ -1291,7 +1303,8 @@
     <col min="26" max="26" width="9.1328125" style="14" customWidth="1"/>
     <col min="27" max="27" width="11.46484375" style="13" customWidth="1"/>
     <col min="28" max="28" width="36.53125" style="2" bestFit="1" customWidth="1"/>
-    <col min="29" max="16384" width="11.46484375" style="2"/>
+    <col min="29" max="29" width="54.86328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="30" max="16384" width="11.46484375" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:30" s="17" customFormat="1" x14ac:dyDescent="0.45">
@@ -1423,19 +1436,19 @@
       <c r="O2" s="17"/>
       <c r="P2" s="17"/>
       <c r="Q2" s="17" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="R2" s="17" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="S2" s="17" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="T2" s="17" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="U2" s="17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="V2" s="17" t="s">
         <v>0</v>
@@ -1447,7 +1460,7 @@
         <v>14</v>
       </c>
       <c r="Y2" s="35" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="Z2" s="17" t="s">
         <v>8</v>
@@ -1456,10 +1469,10 @@
         <v>5</v>
       </c>
       <c r="AB2" s="17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="AC2" s="17" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:30" s="19" customFormat="1" x14ac:dyDescent="0.45">
@@ -1467,7 +1480,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="20" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C3" s="20"/>
       <c r="D3" s="20"/>
@@ -1490,13 +1503,13 @@
       <c r="O3" s="20"/>
       <c r="P3" s="20"/>
       <c r="Q3" s="20" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="R3" s="20" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="S3" s="21" t="s">
-        <v>49</v>
+        <v>76</v>
       </c>
       <c r="T3" s="23"/>
       <c r="U3" s="28"/>
@@ -1506,10 +1519,10 @@
       <c r="W3" s="20"/>
       <c r="X3" s="20"/>
       <c r="Y3" s="33" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="Z3" s="40" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="AA3" s="22"/>
       <c r="AB3" s="22" t="s">
@@ -1525,7 +1538,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
@@ -1541,10 +1554,10 @@
       <c r="O4" s="4"/>
       <c r="P4" s="4"/>
       <c r="Q4" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="R4" s="4" t="s">
         <v>26</v>
-      </c>
-      <c r="R4" s="4" t="s">
-        <v>27</v>
       </c>
       <c r="S4" s="6"/>
       <c r="T4" s="6"/>
@@ -1556,7 +1569,7 @@
       <c r="X4" s="26"/>
       <c r="Y4" s="36"/>
       <c r="Z4" s="41" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="AA4" s="6"/>
       <c r="AB4" s="5" t="s">
@@ -1599,7 +1612,7 @@
       <c r="X5" s="27"/>
       <c r="Y5" s="37"/>
       <c r="Z5" s="42" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="AA5" s="10"/>
       <c r="AB5" s="10" t="s">
@@ -1630,9 +1643,11 @@
       <c r="P6" s="3"/>
       <c r="Q6" s="3"/>
       <c r="R6" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="S6" s="32"/>
+        <v>57</v>
+      </c>
+      <c r="S6" s="44" t="s">
+        <v>74</v>
+      </c>
       <c r="T6" s="12"/>
       <c r="U6" s="3"/>
       <c r="V6" s="12">
@@ -1640,11 +1655,9 @@
       </c>
       <c r="W6" s="3"/>
       <c r="X6" s="3"/>
-      <c r="Y6" s="33" t="s">
-        <v>55</v>
-      </c>
+      <c r="Y6" s="3"/>
       <c r="Z6" s="43" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="AA6" s="3"/>
       <c r="AB6" s="3" t="s">
@@ -1675,21 +1688,21 @@
       <c r="P7" s="24"/>
       <c r="Q7" s="29" t="str">
         <f>DED!$C$4</f>
-        <v>Financial Ceil</v>
+        <v>Financial ceil</v>
       </c>
       <c r="R7" s="29" t="str">
         <f>DED!$D$4</f>
         <v>The person cannot use the power above the amount of</v>
       </c>
-      <c r="S7" s="24" t="str">
+      <c r="S7" s="29" t="str">
         <f>DED!$B$4</f>
-        <v>FINANCIAL CEIL</v>
+        <v>FinancialCeil</v>
       </c>
       <c r="T7" s="24" t="s">
         <v>9</v>
       </c>
       <c r="U7" s="29" t="s">
-        <v>72</v>
+        <v>55</v>
       </c>
       <c r="V7" s="24">
         <v>1</v>
@@ -1702,22 +1715,21 @@
         <f>DED!$F$4</f>
         <v>ccts:Amount</v>
       </c>
-      <c r="Y7" s="34" t="s">
-        <v>56</v>
-      </c>
+      <c r="Y7" s="34"/>
       <c r="Z7" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="AA7" s="29" t="s">
-        <v>1</v>
-      </c>
-      <c r="AB7" s="24" t="str">
+      <c r="AA7" s="29" t="str">
+        <f>IF(DED!$G$4=0,"",DED!$G$4)</f>
+        <v/>
+      </c>
+      <c r="AB7" s="29" t="str">
         <f>IF(DED!$H$4=0,"",DED!$H$4)</f>
-        <v>currencyId compulsory</v>
+        <v>Attribute `currencyId` compulsory when the value is an amount</v>
       </c>
       <c r="AC7" s="29" t="str">
         <f>IF(DED!$I$4=0,"",DED!$I$4)</f>
-        <v/>
+        <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="8" spans="1:30" customFormat="1" x14ac:dyDescent="0.45">
@@ -1741,21 +1753,21 @@
       <c r="P8" s="24"/>
       <c r="Q8" s="29" t="str">
         <f>DED!$C$5</f>
-        <v>Territorial Unit</v>
+        <v>Territorial unit scope</v>
       </c>
       <c r="R8" s="29" t="str">
         <f>DED!$D$5</f>
-        <v>The person can not use the power in the following territorial units</v>
-      </c>
-      <c r="S8" s="24" t="str">
+        <v>The person can not use the power out of the following territorial unit(s)</v>
+      </c>
+      <c r="S8" s="29" t="str">
         <f>DED!$B$5</f>
-        <v>TERRITORIAL_UNIT</v>
+        <v>TerritorialUnitScope</v>
       </c>
       <c r="T8" s="24" t="s">
         <v>9</v>
       </c>
       <c r="U8" s="29" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="V8" s="24" t="s">
         <v>4</v>
@@ -1768,20 +1780,21 @@
         <f>DED!$F$5</f>
         <v>skos:Concept</v>
       </c>
-      <c r="Y8" s="34" t="s">
-        <v>57</v>
-      </c>
+      <c r="Y8" s="34"/>
       <c r="Z8" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="AA8" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="AB8" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="AC8" s="24" t="s">
-        <v>1</v>
+      <c r="AA8" s="29" t="str">
+        <f>IF(DED!$G$5=0,"",DED!$G$5)</f>
+        <v>NUTS-2016</v>
+      </c>
+      <c r="AB8" s="29" t="str">
+        <f>IF(DED!$H$5=0,"",DED!$H$5)</f>
+        <v>Compulsory use of NUTs for the identification of territorial units</v>
+      </c>
+      <c r="AC8" s="29" t="str">
+        <f>IF(DED!$I$5=0,"",DED!$I$5)</f>
+        <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="9" spans="1:30" customFormat="1" x14ac:dyDescent="0.45">
@@ -1805,21 +1818,21 @@
       <c r="P9" s="24"/>
       <c r="Q9" s="29" t="str">
         <f>DED!$C$6</f>
-        <v>Validity Period</v>
+        <v>Validity period</v>
       </c>
       <c r="R9" s="29" t="str">
         <f>DED!$D$6</f>
         <v>The person cannot use the power beyond this time interval</v>
       </c>
-      <c r="S9" s="24" t="str">
+      <c r="S9" s="29" t="str">
         <f>DED!$B$6</f>
-        <v>VALIDITY_PERIOD</v>
+        <v>ValidityPeriodConstraint</v>
       </c>
       <c r="T9" s="24" t="s">
         <v>9</v>
       </c>
       <c r="U9" s="29" t="s">
-        <v>73</v>
+        <v>56</v>
       </c>
       <c r="V9" s="24">
         <v>1</v>
@@ -1832,458 +1845,480 @@
         <f>DED!$F$6</f>
         <v>ubl:Period</v>
       </c>
-      <c r="Y9" s="34" t="s">
-        <v>58</v>
-      </c>
+      <c r="Y9" s="34"/>
       <c r="Z9" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="AA9" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="AB9" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="AC9" s="24" t="s">
-        <v>1</v>
+      <c r="AA9" s="29" t="str">
+        <f>IF(DED!$H$6=0,"",DED!$H$6)</f>
+        <v>If a measure is used to express the length of the period: 1) the endDate must not be specified; and 2) the unitCode of the measure must be specified.</v>
+      </c>
+      <c r="AB9" s="29" t="str">
+        <f>IF(DED!$H$6=0,"",DED!$H$6)</f>
+        <v>If a measure is used to express the length of the period: 1) the endDate must not be specified; and 2) the unitCode of the measure must be specified.</v>
+      </c>
+      <c r="AC9" s="29" t="str">
+        <f>IF(DED!$I$6=0,"",DED!$I$6)</f>
+        <v>Reuse OP's code list</v>
       </c>
     </row>
     <row r="10" spans="1:30" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A10" s="1"/>
       <c r="B10" s="3"/>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="3"/>
+      <c r="D10" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" s="24"/>
+      <c r="F10" s="24"/>
+      <c r="G10" s="24"/>
+      <c r="H10" s="24"/>
+      <c r="I10" s="24"/>
+      <c r="J10" s="24"/>
+      <c r="K10" s="24"/>
+      <c r="L10" s="24"/>
+      <c r="M10" s="24"/>
+      <c r="N10" s="24"/>
+      <c r="O10" s="24"/>
+      <c r="P10" s="24"/>
+      <c r="Q10" s="29" t="str">
+        <f>DED!$C$7</f>
+        <v>One single use</v>
+      </c>
+      <c r="R10" s="29" t="str">
+        <f>DED!$D$7</f>
+        <v>The person cannot use the power more than once</v>
+      </c>
+      <c r="S10" s="29" t="str">
+        <f>DED!$B$7</f>
+        <v>OneSingleUse</v>
+      </c>
+      <c r="T10" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="U10" s="29" t="s">
+        <v>67</v>
+      </c>
+      <c r="V10" s="24">
+        <v>1</v>
+      </c>
+      <c r="W10" s="24" t="str">
+        <f>DED!$E$7</f>
+        <v>IndicatorType</v>
+      </c>
+      <c r="X10" s="24" t="str">
+        <f>DED!$F$7</f>
+        <v>xsd:boolean</v>
+      </c>
+      <c r="Y10" s="34"/>
+      <c r="Z10" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA10" s="29" t="str">
+        <f>IF(DED!$H$7=0,"",DED!$H$7)</f>
+        <v>Once successfully consumed the power, the SP must notify the eMandate Registry so the Registry can change the status of the power.</v>
+      </c>
+      <c r="AB10" s="29" t="str">
+        <f>IF(DED!$H$7=0,"",DED!$H$7)</f>
+        <v>Once successfully consumed the power, the SP must notify the eMandate Registry so the Registry can change the status of the power.</v>
+      </c>
+      <c r="AC10" s="29" t="str">
+        <f>IF(DED!$I$7=0,"",DED!$I$7)</f>
+        <v>If `true`, the maximum number of uses is 1, otherwise it is unlimited</v>
+      </c>
+    </row>
+    <row r="11" spans="1:30" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A11" s="1"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3"/>
-      <c r="L10" s="3"/>
-      <c r="M10" s="3"/>
-      <c r="N10" s="3"/>
-      <c r="O10" s="3"/>
-      <c r="P10" s="3"/>
-      <c r="Q10" s="3"/>
-      <c r="R10" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="S10" s="32"/>
-      <c r="T10" s="12"/>
-      <c r="U10" s="3"/>
-      <c r="V10" s="12">
-        <v>1</v>
-      </c>
-      <c r="W10" s="3"/>
-      <c r="X10" s="3"/>
-      <c r="Y10" s="33" t="s">
-        <v>55</v>
-      </c>
-      <c r="Z10" s="43" t="s">
-        <v>54</v>
-      </c>
-      <c r="AA10" s="3"/>
-      <c r="AB10" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="AC10" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:30" s="19" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="18">
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="3"/>
+      <c r="N11" s="3"/>
+      <c r="O11" s="3"/>
+      <c r="P11" s="3"/>
+      <c r="Q11" s="3"/>
+      <c r="R11" s="11"/>
+      <c r="S11" s="32"/>
+      <c r="T11" s="12"/>
+      <c r="U11" s="3"/>
+      <c r="V11" s="12">
+        <v>1</v>
+      </c>
+      <c r="W11" s="3"/>
+      <c r="X11" s="3"/>
+      <c r="Y11" s="3"/>
+      <c r="Z11" s="3"/>
+      <c r="AA11" s="3"/>
+      <c r="AB11" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="AC11" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:30" s="19" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A12" s="18">
         <v>3</v>
       </c>
-      <c r="B11" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="C11" s="20"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="20" t="s">
-        <v>1</v>
-      </c>
-      <c r="F11" s="20" t="s">
-        <v>1</v>
-      </c>
-      <c r="G11" s="20" t="s">
-        <v>1</v>
-      </c>
-      <c r="H11" s="20"/>
-      <c r="I11" s="20"/>
-      <c r="J11" s="20"/>
-      <c r="K11" s="20"/>
-      <c r="L11" s="20"/>
-      <c r="M11" s="20"/>
-      <c r="N11" s="20"/>
-      <c r="O11" s="20"/>
-      <c r="P11" s="20"/>
-      <c r="Q11" s="20" t="s">
-        <v>34</v>
-      </c>
-      <c r="R11" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="S11" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="T11" s="23"/>
-      <c r="U11" s="28"/>
-      <c r="V11" s="21" t="s">
-        <v>1</v>
-      </c>
-      <c r="W11" s="20"/>
-      <c r="X11" s="20"/>
-      <c r="Y11" s="33" t="s">
-        <v>46</v>
-      </c>
-      <c r="Z11" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="AA11" s="22"/>
-      <c r="AB11" s="22" t="s">
-        <v>1</v>
-      </c>
-      <c r="AC11" s="22"/>
-    </row>
-    <row r="12" spans="1:30" s="19" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A12"/>
-      <c r="B12"/>
-      <c r="C12"/>
-      <c r="D12"/>
-      <c r="E12"/>
-      <c r="F12"/>
-      <c r="G12"/>
-      <c r="H12"/>
-      <c r="I12"/>
-      <c r="J12"/>
-      <c r="K12"/>
-      <c r="L12"/>
-      <c r="M12"/>
-      <c r="N12"/>
-      <c r="O12"/>
-      <c r="P12"/>
-      <c r="Q12"/>
-      <c r="R12"/>
-      <c r="S12"/>
-      <c r="T12"/>
-      <c r="U12"/>
-      <c r="V12"/>
-      <c r="W12"/>
-      <c r="X12"/>
-      <c r="Y12"/>
-      <c r="Z12"/>
-      <c r="AA12"/>
-      <c r="AB12"/>
-      <c r="AC12"/>
-      <c r="AD12"/>
-    </row>
-    <row r="13" spans="1:30" customFormat="1" x14ac:dyDescent="0.45"/>
+      <c r="B12" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="20"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="F12" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="G12" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="H12" s="20"/>
+      <c r="I12" s="20"/>
+      <c r="J12" s="20"/>
+      <c r="K12" s="20"/>
+      <c r="L12" s="20"/>
+      <c r="M12" s="20"/>
+      <c r="N12" s="20"/>
+      <c r="O12" s="20"/>
+      <c r="P12" s="20"/>
+      <c r="Q12" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="R12" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="S12" s="21"/>
+      <c r="T12" s="23"/>
+      <c r="U12" s="28"/>
+      <c r="V12" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="W12" s="20"/>
+      <c r="X12" s="20"/>
+      <c r="Y12" s="20"/>
+      <c r="Z12" s="20"/>
+      <c r="AA12" s="22"/>
+      <c r="AB12" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="AC12" s="22"/>
+    </row>
+    <row r="13" spans="1:30" s="19" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A13"/>
+      <c r="B13"/>
+      <c r="C13"/>
+      <c r="D13"/>
+      <c r="E13"/>
+      <c r="F13"/>
+      <c r="G13"/>
+      <c r="H13"/>
+      <c r="I13"/>
+      <c r="J13"/>
+      <c r="K13"/>
+      <c r="L13"/>
+      <c r="M13"/>
+      <c r="N13"/>
+      <c r="O13"/>
+      <c r="P13"/>
+      <c r="Q13"/>
+      <c r="R13"/>
+      <c r="S13"/>
+      <c r="T13"/>
+      <c r="U13"/>
+      <c r="V13"/>
+      <c r="W13"/>
+      <c r="X13"/>
+      <c r="Y13"/>
+      <c r="Z13"/>
+      <c r="AA13"/>
+      <c r="AB13"/>
+      <c r="AC13"/>
+      <c r="AD13"/>
+    </row>
     <row r="14" spans="1:30" customFormat="1" x14ac:dyDescent="0.45"/>
     <row r="15" spans="1:30" customFormat="1" x14ac:dyDescent="0.45"/>
     <row r="16" spans="1:30" customFormat="1" x14ac:dyDescent="0.45"/>
     <row r="17" spans="1:30" customFormat="1" x14ac:dyDescent="0.45"/>
     <row r="18" spans="1:30" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="19" spans="1:30" s="19" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A19"/>
-      <c r="B19"/>
-      <c r="C19"/>
-      <c r="D19"/>
-      <c r="E19"/>
-      <c r="F19"/>
-      <c r="G19"/>
-      <c r="H19"/>
-      <c r="I19"/>
-      <c r="J19"/>
-      <c r="K19"/>
-      <c r="L19"/>
-      <c r="M19"/>
-      <c r="N19"/>
-      <c r="O19"/>
-      <c r="P19"/>
-      <c r="Q19"/>
-      <c r="R19"/>
-      <c r="S19"/>
-      <c r="T19"/>
-      <c r="U19"/>
-      <c r="V19"/>
-      <c r="W19"/>
-      <c r="X19"/>
-      <c r="Y19"/>
-      <c r="Z19"/>
-      <c r="AA19"/>
-      <c r="AB19"/>
-      <c r="AC19"/>
-      <c r="AD19"/>
-    </row>
-    <row r="20" spans="1:30" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="19" spans="1:30" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="20" spans="1:30" s="19" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A20"/>
+      <c r="B20"/>
+      <c r="C20"/>
+      <c r="D20"/>
+      <c r="E20"/>
+      <c r="F20"/>
+      <c r="G20"/>
+      <c r="H20"/>
+      <c r="I20"/>
+      <c r="J20"/>
+      <c r="K20"/>
+      <c r="L20"/>
+      <c r="M20"/>
+      <c r="N20"/>
+      <c r="O20"/>
+      <c r="P20"/>
+      <c r="Q20"/>
+      <c r="R20"/>
+      <c r="S20"/>
+      <c r="T20"/>
+      <c r="U20"/>
+      <c r="V20"/>
+      <c r="W20"/>
+      <c r="X20"/>
+      <c r="Y20"/>
+      <c r="Z20"/>
+      <c r="AA20"/>
+      <c r="AB20"/>
+      <c r="AC20"/>
+      <c r="AD20"/>
+    </row>
     <row r="21" spans="1:30" customFormat="1" x14ac:dyDescent="0.45"/>
     <row r="22" spans="1:30" customFormat="1" x14ac:dyDescent="0.45"/>
     <row r="23" spans="1:30" customFormat="1" x14ac:dyDescent="0.45"/>
     <row r="24" spans="1:30" customFormat="1" x14ac:dyDescent="0.45"/>
     <row r="25" spans="1:30" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="26" spans="1:30" s="19" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A26"/>
-      <c r="B26"/>
-      <c r="C26"/>
-      <c r="D26"/>
-      <c r="E26"/>
-      <c r="F26"/>
-      <c r="G26"/>
-      <c r="H26"/>
-      <c r="I26"/>
-      <c r="J26"/>
-      <c r="K26"/>
-      <c r="L26"/>
-      <c r="M26"/>
-      <c r="N26"/>
-      <c r="O26"/>
-      <c r="P26"/>
-      <c r="Q26"/>
-      <c r="R26"/>
-      <c r="S26"/>
-      <c r="T26"/>
-      <c r="U26"/>
-      <c r="V26"/>
-      <c r="W26"/>
-      <c r="X26"/>
-      <c r="Y26"/>
-      <c r="Z26"/>
-      <c r="AA26"/>
-      <c r="AB26"/>
-      <c r="AC26"/>
-      <c r="AD26"/>
-    </row>
-    <row r="27" spans="1:30" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="26" spans="1:30" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="27" spans="1:30" s="19" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A27"/>
+      <c r="B27"/>
+      <c r="C27"/>
+      <c r="D27"/>
+      <c r="E27"/>
+      <c r="F27"/>
+      <c r="G27"/>
+      <c r="H27"/>
+      <c r="I27"/>
+      <c r="J27"/>
+      <c r="K27"/>
+      <c r="L27"/>
+      <c r="M27"/>
+      <c r="N27"/>
+      <c r="O27"/>
+      <c r="P27"/>
+      <c r="Q27"/>
+      <c r="R27"/>
+      <c r="S27"/>
+      <c r="T27"/>
+      <c r="U27"/>
+      <c r="V27"/>
+      <c r="W27"/>
+      <c r="X27"/>
+      <c r="Y27"/>
+      <c r="Z27"/>
+      <c r="AA27"/>
+      <c r="AB27"/>
+      <c r="AC27"/>
+      <c r="AD27"/>
+    </row>
     <row r="28" spans="1:30" customFormat="1" x14ac:dyDescent="0.45"/>
     <row r="29" spans="1:30" customFormat="1" x14ac:dyDescent="0.45"/>
     <row r="30" spans="1:30" customFormat="1" x14ac:dyDescent="0.45"/>
     <row r="31" spans="1:30" customFormat="1" x14ac:dyDescent="0.45"/>
     <row r="32" spans="1:30" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="33" spans="1:30" s="19" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A33"/>
-      <c r="B33"/>
-      <c r="C33"/>
-      <c r="D33"/>
-      <c r="E33"/>
-      <c r="F33"/>
-      <c r="G33"/>
-      <c r="H33"/>
-      <c r="I33"/>
-      <c r="J33"/>
-      <c r="K33"/>
-      <c r="L33"/>
-      <c r="M33"/>
-      <c r="N33"/>
-      <c r="O33"/>
-      <c r="P33"/>
-      <c r="Q33"/>
-      <c r="R33"/>
-      <c r="S33"/>
-      <c r="T33"/>
-      <c r="U33"/>
-      <c r="V33"/>
-      <c r="W33"/>
-      <c r="X33"/>
-      <c r="Y33"/>
-      <c r="Z33"/>
-      <c r="AA33"/>
-      <c r="AB33"/>
-      <c r="AC33"/>
-      <c r="AD33"/>
-    </row>
-    <row r="34" spans="1:30" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="33" spans="1:30" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="34" spans="1:30" s="19" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A34"/>
+      <c r="B34"/>
+      <c r="C34"/>
+      <c r="D34"/>
+      <c r="E34"/>
+      <c r="F34"/>
+      <c r="G34"/>
+      <c r="H34"/>
+      <c r="I34"/>
+      <c r="J34"/>
+      <c r="K34"/>
+      <c r="L34"/>
+      <c r="M34"/>
+      <c r="N34"/>
+      <c r="O34"/>
+      <c r="P34"/>
+      <c r="Q34"/>
+      <c r="R34"/>
+      <c r="S34"/>
+      <c r="T34"/>
+      <c r="U34"/>
+      <c r="V34"/>
+      <c r="W34"/>
+      <c r="X34"/>
+      <c r="Y34"/>
+      <c r="Z34"/>
+      <c r="AA34"/>
+      <c r="AB34"/>
+      <c r="AC34"/>
+      <c r="AD34"/>
+    </row>
     <row r="35" spans="1:30" customFormat="1" x14ac:dyDescent="0.45"/>
     <row r="36" spans="1:30" customFormat="1" x14ac:dyDescent="0.45"/>
     <row r="37" spans="1:30" customFormat="1" x14ac:dyDescent="0.45"/>
     <row r="38" spans="1:30" customFormat="1" x14ac:dyDescent="0.45"/>
     <row r="39" spans="1:30" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="40" spans="1:30" s="19" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A40"/>
-      <c r="B40"/>
-      <c r="C40"/>
-      <c r="D40"/>
-      <c r="E40"/>
-      <c r="F40"/>
-      <c r="G40"/>
-      <c r="H40"/>
-      <c r="I40"/>
-      <c r="J40"/>
-      <c r="K40"/>
-      <c r="L40"/>
-      <c r="M40"/>
-      <c r="N40"/>
-      <c r="O40"/>
-      <c r="P40"/>
-      <c r="Q40"/>
-      <c r="R40"/>
-      <c r="S40"/>
-      <c r="T40"/>
-      <c r="U40"/>
-      <c r="V40"/>
-      <c r="W40"/>
-      <c r="X40"/>
-      <c r="Y40"/>
-      <c r="Z40"/>
-      <c r="AA40"/>
-      <c r="AB40"/>
-      <c r="AC40"/>
-      <c r="AD40"/>
-    </row>
-    <row r="41" spans="1:30" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="40" spans="1:30" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="41" spans="1:30" s="19" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A41"/>
+      <c r="B41"/>
+      <c r="C41"/>
+      <c r="D41"/>
+      <c r="E41"/>
+      <c r="F41"/>
+      <c r="G41"/>
+      <c r="H41"/>
+      <c r="I41"/>
+      <c r="J41"/>
+      <c r="K41"/>
+      <c r="L41"/>
+      <c r="M41"/>
+      <c r="N41"/>
+      <c r="O41"/>
+      <c r="P41"/>
+      <c r="Q41"/>
+      <c r="R41"/>
+      <c r="S41"/>
+      <c r="T41"/>
+      <c r="U41"/>
+      <c r="V41"/>
+      <c r="W41"/>
+      <c r="X41"/>
+      <c r="Y41"/>
+      <c r="Z41"/>
+      <c r="AA41"/>
+      <c r="AB41"/>
+      <c r="AC41"/>
+      <c r="AD41"/>
+    </row>
     <row r="42" spans="1:30" customFormat="1" x14ac:dyDescent="0.45"/>
     <row r="43" spans="1:30" customFormat="1" x14ac:dyDescent="0.45"/>
     <row r="44" spans="1:30" customFormat="1" x14ac:dyDescent="0.45"/>
     <row r="45" spans="1:30" customFormat="1" x14ac:dyDescent="0.45"/>
     <row r="46" spans="1:30" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="47" spans="1:30" s="19" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A47"/>
-      <c r="B47"/>
-      <c r="C47"/>
-      <c r="D47"/>
-      <c r="E47"/>
-      <c r="F47"/>
-      <c r="G47"/>
-      <c r="H47"/>
-      <c r="I47"/>
-      <c r="J47"/>
-      <c r="K47"/>
-      <c r="L47"/>
-      <c r="M47"/>
-      <c r="N47"/>
-      <c r="O47"/>
-      <c r="P47"/>
-      <c r="Q47"/>
-      <c r="R47"/>
-      <c r="S47"/>
-      <c r="T47"/>
-      <c r="U47"/>
-      <c r="V47"/>
-      <c r="W47"/>
-      <c r="X47"/>
-      <c r="Y47"/>
-      <c r="Z47"/>
-      <c r="AA47"/>
-      <c r="AB47"/>
-      <c r="AC47"/>
-      <c r="AD47"/>
-    </row>
-    <row r="48" spans="1:30" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="47" spans="1:30" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="48" spans="1:30" s="19" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A48"/>
+      <c r="B48"/>
+      <c r="C48"/>
+      <c r="D48"/>
+      <c r="E48"/>
+      <c r="F48"/>
+      <c r="G48"/>
+      <c r="H48"/>
+      <c r="I48"/>
+      <c r="J48"/>
+      <c r="K48"/>
+      <c r="L48"/>
+      <c r="M48"/>
+      <c r="N48"/>
+      <c r="O48"/>
+      <c r="P48"/>
+      <c r="Q48"/>
+      <c r="R48"/>
+      <c r="S48"/>
+      <c r="T48"/>
+      <c r="U48"/>
+      <c r="V48"/>
+      <c r="W48"/>
+      <c r="X48"/>
+      <c r="Y48"/>
+      <c r="Z48"/>
+      <c r="AA48"/>
+      <c r="AB48"/>
+      <c r="AC48"/>
+      <c r="AD48"/>
+    </row>
     <row r="49" spans="1:30" customFormat="1" x14ac:dyDescent="0.45"/>
     <row r="50" spans="1:30" customFormat="1" x14ac:dyDescent="0.45"/>
     <row r="51" spans="1:30" customFormat="1" x14ac:dyDescent="0.45"/>
     <row r="52" spans="1:30" customFormat="1" x14ac:dyDescent="0.45"/>
     <row r="53" spans="1:30" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="54" spans="1:30" s="19" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A54"/>
-      <c r="B54"/>
-      <c r="C54"/>
-      <c r="D54"/>
-      <c r="E54"/>
-      <c r="F54"/>
-      <c r="G54"/>
-      <c r="H54"/>
-      <c r="I54"/>
-      <c r="J54"/>
-      <c r="K54"/>
-      <c r="L54"/>
-      <c r="M54"/>
-      <c r="N54"/>
-      <c r="O54"/>
-      <c r="P54"/>
-      <c r="Q54"/>
-      <c r="R54"/>
-      <c r="S54"/>
-      <c r="T54"/>
-      <c r="U54"/>
-      <c r="V54"/>
-      <c r="W54"/>
-      <c r="X54"/>
-      <c r="Y54"/>
-      <c r="Z54"/>
-      <c r="AA54"/>
-      <c r="AB54"/>
-      <c r="AC54"/>
-      <c r="AD54"/>
-    </row>
-    <row r="55" spans="1:30" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="54" spans="1:30" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="55" spans="1:30" s="19" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A55"/>
+      <c r="B55"/>
+      <c r="C55"/>
+      <c r="D55"/>
+      <c r="E55"/>
+      <c r="F55"/>
+      <c r="G55"/>
+      <c r="H55"/>
+      <c r="I55"/>
+      <c r="J55"/>
+      <c r="K55"/>
+      <c r="L55"/>
+      <c r="M55"/>
+      <c r="N55"/>
+      <c r="O55"/>
+      <c r="P55"/>
+      <c r="Q55"/>
+      <c r="R55"/>
+      <c r="S55"/>
+      <c r="T55"/>
+      <c r="U55"/>
+      <c r="V55"/>
+      <c r="W55"/>
+      <c r="X55"/>
+      <c r="Y55"/>
+      <c r="Z55"/>
+      <c r="AA55"/>
+      <c r="AB55"/>
+      <c r="AC55"/>
+      <c r="AD55"/>
+    </row>
     <row r="56" spans="1:30" customFormat="1" x14ac:dyDescent="0.45"/>
     <row r="57" spans="1:30" customFormat="1" x14ac:dyDescent="0.45"/>
     <row r="58" spans="1:30" customFormat="1" x14ac:dyDescent="0.45"/>
     <row r="59" spans="1:30" customFormat="1" x14ac:dyDescent="0.45"/>
     <row r="60" spans="1:30" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="61" spans="1:30" s="19" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A61"/>
-      <c r="B61"/>
-      <c r="C61"/>
-      <c r="D61"/>
-      <c r="E61"/>
-      <c r="F61"/>
-      <c r="G61"/>
-      <c r="H61"/>
-      <c r="I61"/>
-      <c r="J61"/>
-      <c r="K61"/>
-      <c r="L61"/>
-      <c r="M61"/>
-      <c r="N61"/>
-      <c r="O61"/>
-      <c r="P61"/>
-      <c r="Q61"/>
-      <c r="R61"/>
-      <c r="S61"/>
-      <c r="T61"/>
-      <c r="U61"/>
-      <c r="V61"/>
-      <c r="W61"/>
-      <c r="X61"/>
-      <c r="Y61"/>
-      <c r="Z61"/>
-      <c r="AA61"/>
-      <c r="AB61"/>
-      <c r="AC61"/>
-      <c r="AD61"/>
-    </row>
-    <row r="62" spans="1:30" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="61" spans="1:30" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="62" spans="1:30" s="19" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A62"/>
+      <c r="B62"/>
+      <c r="C62"/>
+      <c r="D62"/>
+      <c r="E62"/>
+      <c r="F62"/>
+      <c r="G62"/>
+      <c r="H62"/>
+      <c r="I62"/>
+      <c r="J62"/>
+      <c r="K62"/>
+      <c r="L62"/>
+      <c r="M62"/>
+      <c r="N62"/>
+      <c r="O62"/>
+      <c r="P62"/>
+      <c r="Q62"/>
+      <c r="R62"/>
+      <c r="S62"/>
+      <c r="T62"/>
+      <c r="U62"/>
+      <c r="V62"/>
+      <c r="W62"/>
+      <c r="X62"/>
+      <c r="Y62"/>
+      <c r="Z62"/>
+      <c r="AA62"/>
+      <c r="AB62"/>
+      <c r="AC62"/>
+      <c r="AD62"/>
+    </row>
     <row r="63" spans="1:30" customFormat="1" x14ac:dyDescent="0.45"/>
     <row r="64" spans="1:30" customFormat="1" x14ac:dyDescent="0.45"/>
     <row r="65" spans="1:30" customFormat="1" x14ac:dyDescent="0.45"/>
     <row r="66" spans="1:30" customFormat="1" x14ac:dyDescent="0.45"/>
     <row r="67" spans="1:30" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="68" spans="1:30" x14ac:dyDescent="0.45">
-      <c r="A68"/>
-      <c r="B68"/>
-      <c r="C68"/>
-      <c r="D68"/>
-      <c r="E68"/>
-      <c r="F68"/>
-      <c r="G68"/>
-      <c r="H68"/>
-      <c r="I68"/>
-      <c r="J68"/>
-      <c r="K68"/>
-      <c r="L68"/>
-      <c r="M68"/>
-      <c r="N68"/>
-      <c r="O68"/>
-      <c r="P68"/>
-      <c r="Q68"/>
-      <c r="R68"/>
-      <c r="S68"/>
-      <c r="T68"/>
-      <c r="U68"/>
-      <c r="V68"/>
-      <c r="W68"/>
-      <c r="X68"/>
-      <c r="Y68"/>
-      <c r="Z68"/>
-      <c r="AA68"/>
-      <c r="AB68"/>
-      <c r="AC68"/>
-      <c r="AD68"/>
-    </row>
+    <row r="68" spans="1:30" customFormat="1" x14ac:dyDescent="0.45"/>
     <row r="69" spans="1:30" x14ac:dyDescent="0.45">
       <c r="A69"/>
       <c r="B69"/>
@@ -2444,18 +2479,46 @@
       <c r="AC73"/>
       <c r="AD73"/>
     </row>
+    <row r="74" spans="1:30" x14ac:dyDescent="0.45">
+      <c r="A74"/>
+      <c r="B74"/>
+      <c r="C74"/>
+      <c r="D74"/>
+      <c r="E74"/>
+      <c r="F74"/>
+      <c r="G74"/>
+      <c r="H74"/>
+      <c r="I74"/>
+      <c r="J74"/>
+      <c r="K74"/>
+      <c r="L74"/>
+      <c r="M74"/>
+      <c r="N74"/>
+      <c r="O74"/>
+      <c r="P74"/>
+      <c r="Q74"/>
+      <c r="R74"/>
+      <c r="S74"/>
+      <c r="T74"/>
+      <c r="U74"/>
+      <c r="V74"/>
+      <c r="W74"/>
+      <c r="X74"/>
+      <c r="Y74"/>
+      <c r="Z74"/>
+      <c r="AA74"/>
+      <c r="AB74"/>
+      <c r="AC74"/>
+      <c r="AD74"/>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="Y3" r:id="rId1" location="GenericConstraint"/>
-    <hyperlink ref="Y7" r:id="rId2" location="FinancialConstraintProperty"/>
-    <hyperlink ref="Y11" r:id="rId3" location="MaxPaymentThresholdConstraint"/>
-    <hyperlink ref="Y6" r:id="rId4" location="GenericGroup"/>
-    <hyperlink ref="Y8" r:id="rId5" location="GeographicalConstraintProperty"/>
-    <hyperlink ref="Y9" r:id="rId6" location="ValidityPeriodConstraintProperty"/>
-    <hyperlink ref="Y10" r:id="rId7" location="GenericGroup"/>
+    <hyperlink ref="Y12" r:id="rId2" location="MaxPaymentThresholdConstraint" display="https://github.com/everis-rpam/RPaM-Ontology/blob/v1.1.0/06-MorMee_Constraints/mormeeconstraints.ttl#MaxPaymentThresholdConstraint"/>
+    <hyperlink ref="Y11" r:id="rId3" location="GenericGroup" display="https://github.com/everis-rpam/RPaM-Ontology/blob/v1.1.0/06-MorMee_Constraints/mormeeconstraints.ttl#GenericGroup"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId8"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 
@@ -2480,12 +2543,12 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A1" s="25" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B3" s="25" t="s">
         <v>10</v>
@@ -2503,10 +2566,10 @@
         <v>14</v>
       </c>
       <c r="G3" s="25" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H3" s="25" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I3" s="25" t="s">
         <v>15</v>
@@ -2517,22 +2580,25 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>62</v>
+        <v>73</v>
       </c>
       <c r="C4" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D4" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="E4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" t="s">
         <v>18</v>
       </c>
-      <c r="F4" t="s">
-        <v>19</v>
-      </c>
       <c r="H4" t="s">
-        <v>38</v>
+        <v>66</v>
+      </c>
+      <c r="I4" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.45">
@@ -2540,22 +2606,28 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>59</v>
+        <v>72</v>
       </c>
       <c r="C5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D5" t="s">
         <v>60</v>
       </c>
-      <c r="D5" t="s">
-        <v>65</v>
-      </c>
       <c r="E5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F5" t="s">
         <v>16</v>
       </c>
       <c r="G5" t="s">
-        <v>36</v>
+        <v>34</v>
+      </c>
+      <c r="H5" t="s">
+        <v>65</v>
+      </c>
+      <c r="I5" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.45">
@@ -2563,33 +2635,54 @@
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="C6" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="D6" t="s">
-        <v>71</v>
+        <v>54</v>
       </c>
       <c r="E6" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="F6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G6" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="H6" t="s">
-        <v>68</v>
+        <v>51</v>
       </c>
       <c r="I6" t="s">
-        <v>70</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>4</v>
+      </c>
+      <c r="B7" t="s">
+        <v>70</v>
+      </c>
+      <c r="C7" t="s">
+        <v>61</v>
+      </c>
+      <c r="D7" t="s">
+        <v>62</v>
+      </c>
+      <c r="E7" t="s">
+        <v>63</v>
+      </c>
+      <c r="F7" t="s">
+        <v>69</v>
+      </c>
+      <c r="H7" t="s">
+        <v>64</v>
+      </c>
+      <c r="I7" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.45">

</xml_diff>